<commit_message>
visualization of fxnal enrich results for gi hits
</commit_message>
<xml_diff>
--- a/tables/20_45_fxnal-enrich-genetic-interactions/enrichr_results_COAD_A146T.xlsx
+++ b/tables/20_45_fxnal-enrich-genetic-interactions/enrichr_results_COAD_A146T.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="107">
   <si>
     <t>datasource</t>
   </si>
@@ -65,16 +65,70 @@
     <t>8</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>KEA_2015</t>
+  </si>
+  <si>
     <t>PPI_Hub_Proteins</t>
   </si>
   <si>
     <t>WikiPathways_2019_Human</t>
   </si>
   <si>
-    <t>KEA_2015</t>
-  </si>
-  <si>
-    <t>LINCS_L1000_Kinase_Perturbations_down</t>
+    <t>PRKACA</t>
+  </si>
+  <si>
+    <t>PRKG1</t>
   </si>
   <si>
     <t>UBC</t>
@@ -83,22 +137,70 @@
     <t>Regulation of Wnt/B-catenin Signaling by Small Molecule Compounds WP3664</t>
   </si>
   <si>
+    <t>Myometrial Relaxation and Contraction Pathways WP289</t>
+  </si>
+  <si>
+    <t>YWHAZ</t>
+  </si>
+  <si>
+    <t>CDC42</t>
+  </si>
+  <si>
+    <t>CALM3</t>
+  </si>
+  <si>
+    <t>NCK1</t>
+  </si>
+  <si>
     <t>PRKACG</t>
   </si>
   <si>
-    <t>YWHAZ</t>
-  </si>
-  <si>
-    <t>PRKACA</t>
-  </si>
-  <si>
-    <t>CDC42</t>
+    <t>Calcium Regulation in the Cardiac Cell WP536</t>
   </si>
   <si>
     <t>TRAF2</t>
   </si>
   <si>
-    <t>PTK2B_knockdown_96h_A375</t>
+    <t>Interferon type I signaling pathways WP585</t>
+  </si>
+  <si>
+    <t>Association Between Physico-Chemical Features and Toxicity Associated Pathways WP3680</t>
+  </si>
+  <si>
+    <t>CALM1</t>
+  </si>
+  <si>
+    <t>MAPK1</t>
+  </si>
+  <si>
+    <t>FLNA</t>
+  </si>
+  <si>
+    <t>YWHAB</t>
+  </si>
+  <si>
+    <t>YWHAG</t>
+  </si>
+  <si>
+    <t>HSPA1A</t>
+  </si>
+  <si>
+    <t>APC</t>
+  </si>
+  <si>
+    <t>EIF2C2</t>
+  </si>
+  <si>
+    <t>RUVBL2</t>
+  </si>
+  <si>
+    <t>5/393</t>
+  </si>
+  <si>
+    <t>3/106</t>
+  </si>
+  <si>
+    <t>3/121</t>
   </si>
   <si>
     <t>5/540</t>
@@ -107,22 +209,70 @@
     <t>2/17</t>
   </si>
   <si>
+    <t>4/440</t>
+  </si>
+  <si>
+    <t>3/156</t>
+  </si>
+  <si>
+    <t>4/500</t>
+  </si>
+  <si>
+    <t>3/205</t>
+  </si>
+  <si>
+    <t>3/172</t>
+  </si>
+  <si>
+    <t>3/244</t>
+  </si>
+  <si>
     <t>3/176</t>
   </si>
   <si>
-    <t>4/500</t>
-  </si>
-  <si>
-    <t>4/393</t>
-  </si>
-  <si>
-    <t>3/205</t>
+    <t>3/149</t>
   </si>
   <si>
     <t>3/279</t>
   </si>
   <si>
-    <t>4/300</t>
+    <t>2/54</t>
+  </si>
+  <si>
+    <t>2/66</t>
+  </si>
+  <si>
+    <t>3/359</t>
+  </si>
+  <si>
+    <t>3/406</t>
+  </si>
+  <si>
+    <t>2/135</t>
+  </si>
+  <si>
+    <t>4/812</t>
+  </si>
+  <si>
+    <t>3/428</t>
+  </si>
+  <si>
+    <t>2/145</t>
+  </si>
+  <si>
+    <t>2/150</t>
+  </si>
+  <si>
+    <t>2/156</t>
+  </si>
+  <si>
+    <t>2/161</t>
+  </si>
+  <si>
+    <t>RYR1;LRP1;APC;SOX9;SYNE1</t>
+  </si>
+  <si>
+    <t>RYR1;APC;CBL</t>
   </si>
   <si>
     <t>MAP3K1;APC;DAPK1;RGS20;CBL</t>
@@ -131,22 +281,58 @@
     <t>LRP1;APC</t>
   </si>
   <si>
+    <t>RYR1;LRP1;APC;SOX9</t>
+  </si>
+  <si>
+    <t>RYR1;GNAS;RGS20</t>
+  </si>
+  <si>
+    <t>MAP3K1;APC;CBL;SF3B1</t>
+  </si>
+  <si>
+    <t>MAP3K1;CBL;SYNE1</t>
+  </si>
+  <si>
+    <t>RYR1;MAP3K1;DAPK1</t>
+  </si>
+  <si>
+    <t>RYR1;CSDE1;CBL</t>
+  </si>
+  <si>
     <t>LRP1;APC;SOX9</t>
   </si>
   <si>
-    <t>MAP3K1;APC;CBL;SF3B1</t>
-  </si>
-  <si>
-    <t>LRP1;APC;SOX9;SYNE1</t>
-  </si>
-  <si>
-    <t>MAP3K1;CBL;SYNE1</t>
-  </si>
-  <si>
     <t>MAP3K1;PKN1;SOX9</t>
   </si>
   <si>
-    <t>APC;GNAS;SF3B1;SYNE1</t>
+    <t>MAP3K1;CBL</t>
+  </si>
+  <si>
+    <t>APC;CBL</t>
+  </si>
+  <si>
+    <t>MAP3K1;DAPK1;SF3B1</t>
+  </si>
+  <si>
+    <t>MAP3K1;APC</t>
+  </si>
+  <si>
+    <t>LRP1;DAPK1;GNAS;CBL</t>
+  </si>
+  <si>
+    <t>LRP1;CBL;SF3B1</t>
+  </si>
+  <si>
+    <t>MAP3K1;SOX9</t>
+  </si>
+  <si>
+    <t>APC;SYNE1</t>
+  </si>
+  <si>
+    <t>SF3B1;SYNE1</t>
+  </si>
+  <si>
+    <t>MAP3K1;RGS20</t>
   </si>
 </sst>
 </file>
@@ -232,28 +418,28 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="E2" t="n">
-        <v>6.658679941947435E-5</v>
+        <v>1.9814759213675665E-5</v>
       </c>
       <c r="F2" t="n">
-        <v>0.025635917776497624</v>
+        <v>0.008480716943453185</v>
       </c>
       <c r="G2" t="n">
-        <v>10.893246187363834</v>
+        <v>14.13627367825841</v>
       </c>
       <c r="H2" t="n">
-        <v>104.76039441152851</v>
+        <v>153.08288780202616</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="J2" t="n">
         <v>5.0</v>
@@ -264,31 +450,31 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="E3" t="n">
-        <v>9.178965649455299E-5</v>
+        <v>1.1142962034774952E-4</v>
       </c>
       <c r="F3" t="n">
-        <v>0.04332471786542901</v>
+        <v>0.023845938754418396</v>
       </c>
       <c r="G3" t="n">
-        <v>138.4083044982699</v>
+        <v>31.446540880503147</v>
       </c>
       <c r="H3" t="n">
-        <v>1286.6451129463442</v>
+        <v>286.2301061007238</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="J3" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="4">
@@ -296,28 +482,28 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="E4" t="n">
-        <v>4.160011252272865E-4</v>
+        <v>1.6493787707205012E-4</v>
       </c>
       <c r="F4" t="n">
-        <v>0.08902424079863931</v>
+        <v>0.03175054133636965</v>
       </c>
       <c r="G4" t="n">
-        <v>20.053475935828878</v>
+        <v>27.548209366391188</v>
       </c>
       <c r="H4" t="n">
-        <v>156.11275253008125</v>
+        <v>239.94329635130103</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="J4" t="n">
         <v>3.0</v>
@@ -328,31 +514,31 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="E5" t="n">
-        <v>7.089723556156057E-4</v>
+        <v>9.015705300762788E-5</v>
       </c>
       <c r="F5" t="n">
-        <v>0.09098478563733607</v>
+        <v>0.034710465407936736</v>
       </c>
       <c r="G5" t="n">
-        <v>9.411764705882353</v>
+        <v>10.288065843621398</v>
       </c>
       <c r="H5" t="n">
-        <v>68.251237862225</v>
+        <v>95.82260673886584</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="J5" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="6">
@@ -360,31 +546,31 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="E6" t="n">
-        <v>2.8527928057298904E-4</v>
+        <v>1.0321185160705684E-4</v>
       </c>
       <c r="F6" t="n">
-        <v>0.12209953208523931</v>
+        <v>0.04871599395853083</v>
       </c>
       <c r="G6" t="n">
-        <v>11.974255350995362</v>
+        <v>130.718954248366</v>
       </c>
       <c r="H6" t="n">
-        <v>97.7343742036263</v>
+        <v>1199.8335778244314</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="J6" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="7">
@@ -392,31 +578,31 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="E7" t="n">
-        <v>6.490166739074251E-4</v>
+        <v>5.534720449089757E-4</v>
       </c>
       <c r="F7" t="n">
-        <v>0.12493570972717932</v>
+        <v>0.05327168432248891</v>
       </c>
       <c r="G7" t="n">
-        <v>17.216642754662843</v>
+        <v>10.1010101010101</v>
       </c>
       <c r="H7" t="n">
-        <v>126.37105566541055</v>
+        <v>75.75049811239629</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="J7" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="8">
@@ -424,28 +610,28 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0015798341936758746</v>
+        <v>3.485221172083399E-4</v>
       </c>
       <c r="F8" t="n">
-        <v>0.15205904114130292</v>
+        <v>0.05483414644077881</v>
       </c>
       <c r="G8" t="n">
-        <v>12.650221378874132</v>
+        <v>21.36752136752137</v>
       </c>
       <c r="H8" t="n">
-        <v>81.59943552386333</v>
+        <v>170.12412106335466</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="J8" t="n">
         <v>3.0</v>
@@ -456,31 +642,575 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="E9" t="n">
-        <v>1.0121923535514024E-4</v>
+        <v>8.936428005945616E-4</v>
       </c>
       <c r="F9" t="n">
-        <v>0.18442144681706552</v>
+        <v>0.0573420797048177</v>
       </c>
       <c r="G9" t="n">
-        <v>15.686274509803923</v>
+        <v>8.88888888888889</v>
       </c>
       <c r="H9" t="n">
-        <v>144.2858313175401</v>
+        <v>62.401817018138146</v>
       </c>
       <c r="I9" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="J9" t="n">
         <v>4.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="n">
+        <v>7.729597242269839E-4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.059517898765477764</v>
+      </c>
+      <c r="G10" t="n">
+        <v>16.260162601626018</v>
+      </c>
+      <c r="H10" t="n">
+        <v>116.50867664932548</v>
+      </c>
+      <c r="I10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4.6378454079723313E-4</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.05951901606897825</v>
+      </c>
+      <c r="G11" t="n">
+        <v>19.37984496124031</v>
+      </c>
+      <c r="H11" t="n">
+        <v>148.76144312621648</v>
+      </c>
+      <c r="I11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0012780713823151153</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.07029392602733134</v>
+      </c>
+      <c r="G12" t="n">
+        <v>13.66120218579235</v>
+      </c>
+      <c r="H12" t="n">
+        <v>91.0164353808736</v>
+      </c>
+      <c r="I12" t="s">
+        <v>94</v>
+      </c>
+      <c r="J12" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4.959810596683701E-4</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.07075996451268747</v>
+      </c>
+      <c r="G13" t="n">
+        <v>18.939393939393938</v>
+      </c>
+      <c r="H13" t="n">
+        <v>144.10933367653286</v>
+      </c>
+      <c r="I13" t="s">
+        <v>95</v>
+      </c>
+      <c r="J13" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.0459967882687423E-4</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.07188552420314231</v>
+      </c>
+      <c r="G14" t="n">
+        <v>22.371364653243848</v>
+      </c>
+      <c r="H14" t="n">
+        <v>181.1300262172985</v>
+      </c>
+      <c r="I14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.0018763621853418306</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.09029993016957559</v>
+      </c>
+      <c r="G15" t="n">
+        <v>11.947431302270013</v>
+      </c>
+      <c r="H15" t="n">
+        <v>75.01099623038625</v>
+      </c>
+      <c r="I15" t="s">
+        <v>96</v>
+      </c>
+      <c r="J15" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.001064812220373368</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.12564784200405743</v>
+      </c>
+      <c r="G16" t="n">
+        <v>41.15226337448559</v>
+      </c>
+      <c r="H16" t="n">
+        <v>281.6854656076131</v>
+      </c>
+      <c r="I16" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0015859372356271568</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.1497124750432036</v>
+      </c>
+      <c r="G17" t="n">
+        <v>33.670033670033675</v>
+      </c>
+      <c r="H17" t="n">
+        <v>217.0565565844488</v>
+      </c>
+      <c r="I17" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.0038306922932930107</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.16386850365753436</v>
+      </c>
+      <c r="G18" t="n">
+        <v>9.285051067780874</v>
+      </c>
+      <c r="H18" t="n">
+        <v>51.668614082589535</v>
+      </c>
+      <c r="I18" t="s">
+        <v>93</v>
+      </c>
+      <c r="J18" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.005401382602665415</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.17329435850218203</v>
+      </c>
+      <c r="G19" t="n">
+        <v>8.210180623973727</v>
+      </c>
+      <c r="H19" t="n">
+        <v>42.86617668845066</v>
+      </c>
+      <c r="I19" t="s">
+        <v>99</v>
+      </c>
+      <c r="J19" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.0064465840748537725</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.17728106205847877</v>
+      </c>
+      <c r="G20" t="n">
+        <v>16.46090534979424</v>
+      </c>
+      <c r="H20" t="n">
+        <v>83.03217924708406</v>
+      </c>
+      <c r="I20" t="s">
+        <v>100</v>
+      </c>
+      <c r="J20" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.005233309280189198</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.1831658248066219</v>
+      </c>
+      <c r="G21" t="n">
+        <v>5.473453749315818</v>
+      </c>
+      <c r="H21" t="n">
+        <v>28.750473188006232</v>
+      </c>
+      <c r="I21" t="s">
+        <v>101</v>
+      </c>
+      <c r="J21" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.006252390403682648</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.1851669465706015</v>
+      </c>
+      <c r="G22" t="n">
+        <v>7.788161993769471</v>
+      </c>
+      <c r="H22" t="n">
+        <v>39.523297692878046</v>
+      </c>
+      <c r="I22" t="s">
+        <v>102</v>
+      </c>
+      <c r="J22" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.007401409374967147</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.18996950729082346</v>
+      </c>
+      <c r="G23" t="n">
+        <v>15.32567049808429</v>
+      </c>
+      <c r="H23" t="n">
+        <v>75.18903970620426</v>
+      </c>
+      <c r="I23" t="s">
+        <v>103</v>
+      </c>
+      <c r="J23" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.007901474565627706</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.19012923173541668</v>
+      </c>
+      <c r="G24" t="n">
+        <v>14.814814814814817</v>
+      </c>
+      <c r="H24" t="n">
+        <v>71.71416123036896</v>
+      </c>
+      <c r="I24" t="s">
+        <v>104</v>
+      </c>
+      <c r="J24" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.008521247395824046</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.19298119102307398</v>
+      </c>
+      <c r="G25" t="n">
+        <v>14.245014245014245</v>
+      </c>
+      <c r="H25" t="n">
+        <v>67.88023562531258</v>
+      </c>
+      <c r="I25" t="s">
+        <v>105</v>
+      </c>
+      <c r="J25" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.00905398591923573</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.19365469882809755</v>
+      </c>
+      <c r="G26" t="n">
+        <v>13.80262249827467</v>
+      </c>
+      <c r="H26" t="n">
+        <v>64.93513023005872</v>
+      </c>
+      <c r="I26" t="s">
+        <v>106</v>
+      </c>
+      <c r="J26" t="n">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>